<commit_message>
create new Test packet and create new many Excel class
</commit_message>
<xml_diff>
--- a/Employees.xlsx
+++ b/Employees.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cybertekb24/IdeaProjects/CucumberProjectB24/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DAD28BC-FD6C-2748-B535-5C3B8A369DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6700" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{3463B30F-B23A-1844-91CB-48DD17889895}"/>
+    <workbookView xWindow="375" yWindow="495" windowWidth="28035" windowHeight="16095"/>
   </bookViews>
   <sheets>
-    <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>FirstName</t>
   </si>
@@ -73,7 +74,7 @@
     <t>Fahima</t>
   </si>
   <si>
-    <t>Eldarrat</t>
+    <t>Eldarat</t>
   </si>
   <si>
     <t>CTO</t>
@@ -104,12 +105,16 @@
   </si>
   <si>
     <t>Co-Founder</t>
+  </si>
+  <si>
+    <t>Salary</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -454,21 +459,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48EA3C76-4832-6F42-AF56-331A33D59B87}">
-  <dimension ref="A1:C8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="242" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="15.1640625" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -478,8 +478,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -489,8 +492,11 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="n">
+        <v>111000.0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -500,8 +506,11 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="n">
+        <v>118000.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -511,8 +520,11 @@
       <c r="C4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="n">
+        <v>148000.0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -523,7 +535,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -534,7 +546,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -545,7 +557,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>

</xml_diff>